<commit_message>
Refactor - validate Icthama EPV component. Update Proto
</commit_message>
<xml_diff>
--- a/tabular/genus/proto-refseqs-side-data.xlsx
+++ b/tabular/genus/proto-refseqs-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/genus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC459105-F0EF-F44C-BB99-1D110C34227C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD829E8-FC67-CB4E-B016-4BA0E200E92B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5260" yWindow="8760" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15660" yWindow="4600" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Refset" sheetId="4" r:id="rId1"/>
@@ -2547,12 +2547,12 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A3:A16"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="3" max="3" width="48.33203125" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
     <col min="5" max="5" width="21.33203125" customWidth="1"/>

</xml_diff>